<commit_message>
analysed VFH and VTV
</commit_message>
<xml_diff>
--- a/etf_analysis/NLR/NLR_backtest_results.xlsx
+++ b/etf_analysis/NLR/NLR_backtest_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyin1\OneDrive\uni-hers\Projects and Competitions\Citi 24\Citi-Comp-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyin1\OneDrive\uni-hers\Projects and Competitions\Citi 24\Citi-Comp-24\etf_analysis\NLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34DB985-0987-4C7E-9FEB-026801F10A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33212B2F-1F7B-4DC3-8937-30D9B7274905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,10 +105,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -157,10 +157,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Actual Price</c:v>
+            <c:v>Historical Price</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="3A3A3A"/>
               </a:solidFill>
@@ -1328,10 +1328,10 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Predicted Price</c:v>
+            <c:v>Model Predicted Price</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="3742AE"/>
               </a:solidFill>
@@ -2566,20 +2566,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3323,14 +3309,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>160053</xdr:rowOff>
+      <xdr:rowOff>160054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3647,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>